<commit_message>
Added data driven test case and updated conftest to supress save password popup
</commit_message>
<xml_diff>
--- a/testdata/LoginData.xlsx
+++ b/testdata/LoginData.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1030666\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Old D drive\SeleniumWorkSpace\nop_commerce_pytest_framework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="login_data_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>adm@yourtore.com</t>
+  </si>
+  <si>
+    <t>admin@youtore.com</t>
   </si>
 </sst>
 </file>
@@ -379,7 +385,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,7 +419,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -424,7 +430,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>

</xml_diff>